<commit_message>
updated with all the milestones
</commit_message>
<xml_diff>
--- a/Task Sheet/Samsara Task Sheet.xlsx
+++ b/Task Sheet/Samsara Task Sheet.xlsx
@@ -301,6 +301,9 @@
     <t>HTML retrofitting</t>
   </si>
   <si>
+    <t>Sign Up</t>
+  </si>
+  <si>
     <t>Add Service</t>
   </si>
   <si>
@@ -316,7 +319,76 @@
     <t>Volunteer dashboard</t>
   </si>
   <si>
+    <t>UX Design</t>
+  </si>
+  <si>
+    <t>Front End</t>
+  </si>
+  <si>
+    <t>HTML retrofitting</t>
+  </si>
+  <si>
+    <t>Sign Up</t>
+  </si>
+  <si>
+    <t>Calendar &amp; Activities</t>
+  </si>
+  <si>
+    <t>Edit Profile</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
     <t>Admin Module</t>
+  </si>
+  <si>
+    <t>UX Design</t>
+  </si>
+  <si>
+    <t>Front End</t>
+  </si>
+  <si>
+    <t>HTML retrofitting</t>
+  </si>
+  <si>
+    <t>Approve Users</t>
+  </si>
+  <si>
+    <t>Create Sub Admin</t>
+  </si>
+  <si>
+    <t>Abuse Reports</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Ban User</t>
+  </si>
+  <si>
+    <t>Manage Articles</t>
+  </si>
+  <si>
+    <t>Manage Service Providers</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t>Manage Products</t>
+  </si>
+  <si>
+    <t>Manage Discussions</t>
+  </si>
+  <si>
+    <t>PARKED</t>
+  </si>
+  <si>
+    <t>Manage volunteers</t>
+  </si>
+  <si>
+    <t>Create Events</t>
   </si>
 </sst>
 </file>
@@ -1279,7 +1351,9 @@
       <c t="s" s="2" r="D82">
         <v>96</v>
       </c>
-      <c s="2" r="E82"/>
+      <c s="2" r="E82">
+        <v>24.0</v>
+      </c>
     </row>
     <row r="83">
       <c s="2" r="A83"/>
@@ -1287,7 +1361,9 @@
       <c t="s" s="2" r="D83">
         <v>97</v>
       </c>
-      <c s="2" r="E83"/>
+      <c s="2" r="E83">
+        <v>24.0</v>
+      </c>
     </row>
     <row r="84">
       <c s="2" r="A84"/>
@@ -1295,7 +1371,9 @@
       <c t="s" s="2" r="D84">
         <v>98</v>
       </c>
-      <c s="2" r="E84"/>
+      <c s="2" r="E84">
+        <v>24.0</v>
+      </c>
     </row>
     <row r="85">
       <c s="2" r="A85"/>
@@ -1303,20 +1381,26 @@
       <c t="s" s="2" r="D85">
         <v>99</v>
       </c>
-      <c s="2" r="E85"/>
+      <c s="2" r="E85">
+        <v>36.0</v>
+      </c>
     </row>
     <row r="86">
       <c s="2" r="A86"/>
       <c s="2" r="C86"/>
-      <c s="2" r="D86"/>
-      <c s="2" r="E86"/>
+      <c t="s" s="2" r="D86">
+        <v>100</v>
+      </c>
+      <c s="2" r="E86">
+        <v>24.0</v>
+      </c>
     </row>
     <row r="87">
       <c s="2" r="A87">
         <v>9.0</v>
       </c>
       <c t="s" s="2" r="B87">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c s="2" r="C87"/>
       <c s="2" r="D87"/>
@@ -1324,55 +1408,66 @@
     </row>
     <row r="88">
       <c s="2" r="A88"/>
-      <c s="2" r="C88"/>
+      <c t="s" s="2" r="C88">
+        <v>102</v>
+      </c>
       <c s="2" r="D88"/>
       <c s="2" r="E88"/>
     </row>
     <row r="89">
-      <c s="2" r="A89">
-        <v>10.0</v>
-      </c>
-      <c t="s" s="2" r="B89">
-        <v>101</v>
-      </c>
-      <c s="2" r="C89"/>
+      <c s="2" r="A89"/>
+      <c t="s" s="2" r="C89">
+        <v>103</v>
+      </c>
       <c s="2" r="D89"/>
       <c s="2" r="E89"/>
     </row>
     <row r="90">
       <c s="2" r="A90"/>
-      <c s="2" r="B90"/>
-      <c s="2" r="C90"/>
+      <c t="s" s="2" r="C90">
+        <v>104</v>
+      </c>
       <c s="2" r="D90"/>
       <c s="2" r="E90"/>
     </row>
     <row r="91">
       <c s="2" r="A91"/>
-      <c s="2" r="B91"/>
-      <c s="2" r="C91"/>
-      <c s="2" r="D91"/>
-      <c s="2" r="E91"/>
+      <c t="s" s="2" r="D91">
+        <v>105</v>
+      </c>
+      <c s="2" r="E91">
+        <v>24.0</v>
+      </c>
     </row>
     <row r="92">
       <c s="2" r="A92"/>
-      <c s="2" r="B92"/>
       <c s="2" r="C92"/>
-      <c s="2" r="D92"/>
-      <c s="2" r="E92"/>
+      <c t="s" s="2" r="D92">
+        <v>106</v>
+      </c>
+      <c s="2" r="E92">
+        <v>36.0</v>
+      </c>
     </row>
     <row r="93">
-      <c s="2" r="A93"/>
-      <c s="2" r="B93"/>
       <c s="2" r="C93"/>
-      <c s="2" r="D93"/>
-      <c s="2" r="E93"/>
+      <c t="s" s="2" r="D93">
+        <v>107</v>
+      </c>
+      <c s="2" r="E93">
+        <v>36.0</v>
+      </c>
     </row>
     <row r="94">
       <c s="2" r="A94"/>
       <c s="2" r="B94"/>
       <c s="2" r="C94"/>
-      <c s="2" r="D94"/>
-      <c s="2" r="E94"/>
+      <c t="s" s="2" r="D94">
+        <v>108</v>
+      </c>
+      <c s="2" r="E94">
+        <v>24.0</v>
+      </c>
     </row>
     <row r="95">
       <c s="2" r="A95"/>
@@ -1382,8 +1477,12 @@
       <c s="2" r="E95"/>
     </row>
     <row r="96">
-      <c s="2" r="A96"/>
-      <c s="2" r="B96"/>
+      <c s="2" r="A96">
+        <v>10.0</v>
+      </c>
+      <c t="s" s="2" r="B96">
+        <v>109</v>
+      </c>
       <c s="2" r="C96"/>
       <c s="2" r="D96"/>
       <c s="2" r="E96"/>
@@ -1391,21 +1490,27 @@
     <row r="97">
       <c s="2" r="A97"/>
       <c s="2" r="B97"/>
-      <c s="2" r="C97"/>
+      <c t="s" s="2" r="C97">
+        <v>110</v>
+      </c>
       <c s="2" r="D97"/>
       <c s="2" r="E97"/>
     </row>
     <row r="98">
       <c s="2" r="A98"/>
       <c s="2" r="B98"/>
-      <c s="2" r="C98"/>
+      <c t="s" s="2" r="C98">
+        <v>111</v>
+      </c>
       <c s="2" r="D98"/>
       <c s="2" r="E98"/>
     </row>
     <row r="99">
       <c s="2" r="A99"/>
       <c s="2" r="B99"/>
-      <c s="2" r="C99"/>
+      <c t="s" s="2" r="C99">
+        <v>112</v>
+      </c>
       <c s="2" r="D99"/>
       <c s="2" r="E99"/>
     </row>
@@ -1413,78 +1518,140 @@
       <c s="2" r="A100"/>
       <c s="2" r="B100"/>
       <c s="2" r="C100"/>
-      <c s="2" r="D100"/>
-      <c s="2" r="E100"/>
+      <c t="s" s="2" r="D100">
+        <v>113</v>
+      </c>
+      <c s="2" r="E100">
+        <v>36.0</v>
+      </c>
     </row>
     <row r="101">
       <c s="2" r="A101"/>
       <c s="2" r="B101"/>
       <c s="2" r="C101"/>
-      <c s="2" r="D101"/>
-      <c s="2" r="E101"/>
+      <c t="s" s="2" r="D101">
+        <v>114</v>
+      </c>
+      <c s="2" r="E101">
+        <v>24.0</v>
+      </c>
     </row>
     <row r="102">
       <c s="2" r="A102"/>
       <c s="2" r="B102"/>
       <c s="2" r="C102"/>
-      <c s="2" r="D102"/>
-      <c s="2" r="E102"/>
+      <c t="s" s="2" r="D102">
+        <v>115</v>
+      </c>
+      <c s="2" r="E102">
+        <v>24.0</v>
+      </c>
     </row>
     <row r="103">
       <c s="2" r="A103"/>
       <c s="2" r="B103"/>
       <c s="2" r="C103"/>
-      <c s="2" r="D103"/>
-      <c s="2" r="E103"/>
+      <c t="s" s="2" r="D103">
+        <v>116</v>
+      </c>
+      <c s="2" r="E103">
+        <v>24.0</v>
+      </c>
     </row>
     <row r="104">
       <c s="2" r="A104"/>
       <c s="2" r="B104"/>
       <c s="2" r="C104"/>
-      <c s="2" r="D104"/>
-      <c s="2" r="E104"/>
+      <c t="s" s="2" r="D104">
+        <v>117</v>
+      </c>
+      <c s="2" r="E104">
+        <v>24.0</v>
+      </c>
     </row>
     <row r="105">
-      <c s="2" r="D105"/>
-      <c s="2" r="E105"/>
+      <c s="2" r="A105"/>
+      <c s="2" r="B105"/>
+      <c s="2" r="C105"/>
+      <c t="s" s="2" r="D105">
+        <v>118</v>
+      </c>
+      <c s="2" r="E105">
+        <v>24.0</v>
+      </c>
     </row>
     <row r="106">
-      <c s="2" r="D106"/>
-      <c s="2" r="E106"/>
+      <c s="2" r="A106"/>
+      <c s="2" r="B106"/>
+      <c s="2" r="C106"/>
+      <c t="s" s="2" r="D106">
+        <v>119</v>
+      </c>
+      <c s="2" r="E106">
+        <v>24.0</v>
+      </c>
     </row>
     <row r="107">
-      <c s="2" r="D107"/>
-      <c s="2" r="E107"/>
+      <c t="s" s="2" r="D107">
+        <v>120</v>
+      </c>
+      <c s="2" r="E107">
+        <v>24.0</v>
+      </c>
     </row>
     <row r="108">
-      <c s="2" r="D108"/>
-      <c s="2" r="E108"/>
+      <c t="s" s="2" r="D108">
+        <v>121</v>
+      </c>
+      <c s="2" r="E108">
+        <v>24.0</v>
+      </c>
     </row>
     <row r="109">
-      <c s="2" r="D109"/>
-      <c s="2" r="E109"/>
+      <c t="s" s="2" r="D109">
+        <v>122</v>
+      </c>
+      <c t="s" s="2" r="E109">
+        <v>123</v>
+      </c>
     </row>
     <row r="110">
-      <c s="2" r="D110"/>
-      <c s="2" r="E110"/>
+      <c t="s" s="2" r="D110">
+        <v>124</v>
+      </c>
+      <c s="2" r="E110">
+        <v>24.0</v>
+      </c>
     </row>
     <row r="111">
-      <c s="2" r="E111"/>
+      <c t="s" s="2" r="D111">
+        <v>125</v>
+      </c>
+      <c s="2" r="E111">
+        <v>24.0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c s="2" r="D112"/>
+      <c s="2" r="E112"/>
     </row>
     <row r="113">
       <c s="2" r="E113"/>
     </row>
-    <row r="114">
-      <c s="2" r="E114"/>
-    </row>
-    <row r="118">
-      <c s="2" r="A118"/>
-      <c s="2" r="B118"/>
-      <c s="2" r="C118"/>
-      <c s="2" r="D118"/>
-    </row>
-    <row r="119">
-      <c s="2" r="D119"/>
+    <row r="115">
+      <c s="2" r="E115"/>
+    </row>
+    <row r="116">
+      <c s="2" r="E116"/>
+    </row>
+    <row r="120">
+      <c s="2" r="A120"/>
+      <c s="2" r="B120"/>
+      <c s="2" r="C120"/>
+      <c s="2" r="D120"/>
+    </row>
+    <row r="121">
+      <c s="2" r="D121"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>